<commit_message>
That's all folks - final edit of JS-SPA-Self-Evaluation-Protocol.xlsx
</commit_message>
<xml_diff>
--- a/AngularSpaAdds/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/AngularSpaAdds/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>https://github.com/g-stoyanov</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -841,7 +844,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -1064,7 +1067,9 @@
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1074,7 +1079,9 @@
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1091,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1245,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>